<commit_message>
Update BGDP in other files that rely on those data
</commit_message>
<xml_diff>
--- a/InputData/elec/DCpUC/Decommissioning Cost per Unit Cap.xlsx
+++ b/InputData/elec/DCpUC/Decommissioning Cost per Unit Cap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\DCpUC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\DCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -718,7 +718,7 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>3.2347480211350491E-2</v>
+        <v>3.878298458735905E-2</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +965,7 @@
       </c>
       <c r="B2" s="6">
         <f>Data!C3*About!$A$33</f>
-        <v>3620.4532471238008</v>
+        <v>4340.7394197334379</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -974,7 +974,7 @@
       </c>
       <c r="B3" s="6">
         <f>Data!C8*About!$A$33</f>
-        <v>464.16067270817956</v>
+        <v>556.50505381197922</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -983,7 +983,7 @@
       </c>
       <c r="B4" s="6">
         <f>Data!C13*About!$A$33</f>
-        <v>23966.162734165671</v>
+        <v>28734.210945158524</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -992,7 +992,7 @@
       </c>
       <c r="B5" s="6">
         <f>Data!B19*About!$A$33</f>
-        <v>21151.437870871141</v>
+        <v>25359.498903368527</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B6" s="6">
         <f>Data!C6*About!$A$33</f>
-        <v>1578.1462872078107</v>
+        <v>1892.1171829607295</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B7" s="6">
         <f>Data!C5*About!$A$33</f>
-        <v>1763.8105562910823</v>
+        <v>2114.719204485521</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="B8" s="6">
         <f>Data!C4*About!$A$33</f>
-        <v>2908.7402156379258</v>
+        <v>3487.43167055507</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="B9" s="9">
         <f>Data!C3*About!$A$33</f>
-        <v>3620.4532471238008</v>
+        <v>4340.7394197334379</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B10" s="11">
         <f>B5*About!$A$33</f>
-        <v>684.19571796961361</v>
+        <v>983.51705511249031</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B11" s="6">
         <f>Data!C7*About!$A$33</f>
-        <v>959.26539026357113</v>
+        <v>1150.110444544757</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="B12" s="6">
         <f>Data!C8*About!$A$33</f>
-        <v>464.16067270817956</v>
+        <v>556.50505381197922</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B13" s="6">
         <f>Data!C3*About!$A$33</f>
-        <v>3620.4532471238008</v>
+        <v>4340.7394197334379</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="B14" s="6">
         <f>Data!C2*About!$A$33</f>
-        <v>6560.137507608938</v>
+        <v>7865.2714272093062</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="B15" s="6">
         <f>B11*About!$A$33</f>
-        <v>31.029818228984272</v>
+        <v>44.604715644539979</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B16" s="6">
         <f>B11*About!$A$33</f>
-        <v>31.029818228984272</v>
+        <v>44.604715644539979</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -1100,7 +1100,7 @@
       </c>
       <c r="B17" s="6">
         <f>B9*About!$A$33</f>
-        <v>117.11253976745677</v>
+        <v>168.3468300132638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>